<commit_message>
Some major changes, LOs cleaned. AJAX logic cleanup is yet to be done.
</commit_message>
<xml_diff>
--- a/lolist_APhy.xlsx
+++ b/lolist_APhy.xlsx
@@ -26,21 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="258">
   <si>
-    <t>Topic</t>
-  </si>
-  <si>
-    <t>LO Code</t>
-  </si>
-  <si>
-    <t>LO Description</t>
-  </si>
-  <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>Grade</t>
-  </si>
-  <si>
     <t>Physics</t>
   </si>
   <si>
@@ -798,6 +783,21 @@
   </si>
   <si>
     <t>Explain how Hubble’s law supports the Big Bang theory</t>
+  </si>
+  <si>
+    <t>grade</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>lo_code</t>
+  </si>
+  <si>
+    <t>lo_description</t>
   </si>
 </sst>
 </file>
@@ -1117,1568 +1117,1568 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="A133" sqref="A133"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>253</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>254</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>255</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>256</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
         <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
         <v>43</v>
       </c>
-      <c r="B8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
         <v>57</v>
       </c>
-      <c r="B16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" t="s">
-        <v>5</v>
-      </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="E20" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" t="s">
         <v>66</v>
       </c>
-      <c r="B21" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" t="s">
-        <v>5</v>
-      </c>
       <c r="E21" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="E23" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D24" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
       <c r="E24" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" t="s">
         <v>73</v>
       </c>
-      <c r="B25" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" t="s">
-        <v>79</v>
-      </c>
-      <c r="D25" t="s">
-        <v>5</v>
-      </c>
       <c r="E25" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="E27" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>83</v>
+        <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D28" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="E28" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="C30" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D30" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="E30" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D31" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="E31" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" t="s">
         <v>85</v>
       </c>
-      <c r="B32" t="s">
-        <v>90</v>
-      </c>
-      <c r="C32" t="s">
-        <v>91</v>
-      </c>
-      <c r="D32" t="s">
-        <v>5</v>
-      </c>
       <c r="E32" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>92</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>93</v>
+        <v>0</v>
       </c>
       <c r="C34" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D34" t="s">
-        <v>5</v>
+        <v>88</v>
       </c>
       <c r="E34" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>92</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D35" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="E35" t="s">
-        <v>38</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="B37" t="s">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="C37" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D37" t="s">
-        <v>5</v>
+        <v>93</v>
       </c>
       <c r="E37" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="B38" t="s">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C38" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D38" t="s">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="E38" t="s">
-        <v>38</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>102</v>
+        <v>33</v>
       </c>
       <c r="B40" t="s">
-        <v>103</v>
+        <v>0</v>
       </c>
       <c r="C40" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D40" t="s">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="E40" t="s">
-        <v>38</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>102</v>
+        <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="C41" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D41" t="s">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="E41" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>107</v>
+        <v>33</v>
       </c>
       <c r="B43" t="s">
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="C43" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D43" t="s">
-        <v>5</v>
+        <v>103</v>
       </c>
       <c r="E43" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>107</v>
+        <v>33</v>
       </c>
       <c r="B44" t="s">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="C44" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="D44" t="s">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="E44" t="s">
-        <v>38</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" t="s">
+        <v>102</v>
+      </c>
+      <c r="D45" t="s">
         <v>107</v>
       </c>
-      <c r="B45" t="s">
-        <v>112</v>
-      </c>
-      <c r="C45" t="s">
-        <v>113</v>
-      </c>
-      <c r="D45" t="s">
-        <v>5</v>
-      </c>
       <c r="E45" t="s">
-        <v>38</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>114</v>
+        <v>33</v>
       </c>
       <c r="B47" t="s">
-        <v>115</v>
+        <v>0</v>
       </c>
       <c r="C47" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D47" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="E47" t="s">
-        <v>38</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>114</v>
+        <v>33</v>
       </c>
       <c r="B48" t="s">
-        <v>117</v>
+        <v>0</v>
       </c>
       <c r="C48" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D48" t="s">
-        <v>5</v>
+        <v>112</v>
       </c>
       <c r="E48" t="s">
-        <v>38</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>119</v>
+        <v>33</v>
       </c>
       <c r="B50" t="s">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C50" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D50" t="s">
-        <v>5</v>
+        <v>115</v>
       </c>
       <c r="E50" t="s">
-        <v>38</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>119</v>
+        <v>33</v>
       </c>
       <c r="B51" t="s">
-        <v>122</v>
+        <v>0</v>
       </c>
       <c r="C51" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D51" t="s">
-        <v>5</v>
+        <v>117</v>
       </c>
       <c r="E51" t="s">
-        <v>38</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>124</v>
+        <v>33</v>
       </c>
       <c r="B53" t="s">
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="C53" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D53" t="s">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="E53" t="s">
-        <v>38</v>
+        <v>121</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>124</v>
+        <v>33</v>
       </c>
       <c r="B54" t="s">
-        <v>127</v>
+        <v>0</v>
       </c>
       <c r="C54" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D54" t="s">
-        <v>5</v>
+        <v>122</v>
       </c>
       <c r="E54" t="s">
-        <v>38</v>
+        <v>123</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>33</v>
+      </c>
+      <c r="B55" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>119</v>
+      </c>
+      <c r="D55" t="s">
         <v>124</v>
       </c>
-      <c r="B55" t="s">
-        <v>129</v>
-      </c>
-      <c r="C55" t="s">
-        <v>130</v>
-      </c>
-      <c r="D55" t="s">
-        <v>5</v>
-      </c>
       <c r="E55" t="s">
-        <v>38</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>131</v>
+        <v>33</v>
       </c>
       <c r="B57" t="s">
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="C57" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D57" t="s">
-        <v>5</v>
+        <v>127</v>
       </c>
       <c r="E57" t="s">
-        <v>38</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>131</v>
+        <v>33</v>
       </c>
       <c r="B58" t="s">
-        <v>134</v>
+        <v>0</v>
       </c>
       <c r="C58" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D58" t="s">
-        <v>5</v>
+        <v>129</v>
       </c>
       <c r="E58" t="s">
-        <v>38</v>
+        <v>130</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>136</v>
+        <v>33</v>
       </c>
       <c r="B60" t="s">
-        <v>137</v>
+        <v>0</v>
       </c>
       <c r="C60" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D60" t="s">
-        <v>5</v>
+        <v>132</v>
       </c>
       <c r="E60" t="s">
-        <v>38</v>
+        <v>133</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>136</v>
+        <v>33</v>
       </c>
       <c r="B61" t="s">
-        <v>139</v>
+        <v>0</v>
       </c>
       <c r="C61" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D61" t="s">
-        <v>5</v>
+        <v>134</v>
       </c>
       <c r="E61" t="s">
-        <v>38</v>
+        <v>135</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>141</v>
+        <v>33</v>
       </c>
       <c r="B63" t="s">
-        <v>142</v>
+        <v>0</v>
       </c>
       <c r="C63" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D63" t="s">
-        <v>5</v>
+        <v>137</v>
       </c>
       <c r="E63" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>141</v>
+        <v>33</v>
       </c>
       <c r="B64" t="s">
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="C64" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D64" t="s">
-        <v>5</v>
+        <v>139</v>
       </c>
       <c r="E64" t="s">
-        <v>38</v>
+        <v>140</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>146</v>
+        <v>33</v>
       </c>
       <c r="B66" t="s">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="C66" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D66" t="s">
-        <v>5</v>
+        <v>142</v>
       </c>
       <c r="E66" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>146</v>
+        <v>33</v>
       </c>
       <c r="B67" t="s">
-        <v>149</v>
+        <v>0</v>
       </c>
       <c r="C67" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D67" t="s">
-        <v>5</v>
+        <v>144</v>
       </c>
       <c r="E67" t="s">
-        <v>38</v>
+        <v>145</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>151</v>
+        <v>33</v>
       </c>
       <c r="B69" t="s">
-        <v>152</v>
+        <v>0</v>
       </c>
       <c r="C69" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D69" t="s">
-        <v>5</v>
+        <v>147</v>
       </c>
       <c r="E69" t="s">
-        <v>38</v>
+        <v>148</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>154</v>
+        <v>33</v>
       </c>
       <c r="B71" t="s">
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="C71" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="D71" t="s">
-        <v>5</v>
+        <v>150</v>
       </c>
       <c r="E71" t="s">
-        <v>38</v>
+        <v>151</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>157</v>
+        <v>33</v>
       </c>
       <c r="B73" t="s">
-        <v>158</v>
+        <v>0</v>
       </c>
       <c r="C73" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="D73" t="s">
-        <v>5</v>
+        <v>153</v>
       </c>
       <c r="E73" t="s">
-        <v>38</v>
+        <v>154</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>157</v>
+        <v>33</v>
       </c>
       <c r="B74" t="s">
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="C74" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="D74" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="E74" t="s">
-        <v>38</v>
+        <v>156</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>162</v>
+        <v>33</v>
       </c>
       <c r="B76" t="s">
-        <v>163</v>
+        <v>0</v>
       </c>
       <c r="C76" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D76" t="s">
-        <v>5</v>
+        <v>158</v>
       </c>
       <c r="E76" t="s">
-        <v>38</v>
+        <v>159</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>162</v>
+        <v>33</v>
       </c>
       <c r="B77" t="s">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="C77" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D77" t="s">
-        <v>5</v>
+        <v>160</v>
       </c>
       <c r="E77" t="s">
-        <v>38</v>
+        <v>161</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>167</v>
+        <v>33</v>
       </c>
       <c r="B79" t="s">
-        <v>168</v>
+        <v>0</v>
       </c>
       <c r="C79" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D79" t="s">
-        <v>5</v>
+        <v>163</v>
       </c>
       <c r="E79" t="s">
-        <v>38</v>
+        <v>164</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>170</v>
+        <v>33</v>
       </c>
       <c r="B81" t="s">
-        <v>171</v>
+        <v>0</v>
       </c>
       <c r="C81" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D81" t="s">
-        <v>5</v>
+        <v>166</v>
       </c>
       <c r="E81" t="s">
-        <v>38</v>
+        <v>167</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>170</v>
+        <v>33</v>
       </c>
       <c r="B82" t="s">
-        <v>173</v>
+        <v>0</v>
       </c>
       <c r="C82" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="D82" t="s">
-        <v>5</v>
+        <v>168</v>
       </c>
       <c r="E82" t="s">
-        <v>38</v>
+        <v>169</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>175</v>
+        <v>33</v>
       </c>
       <c r="B84" t="s">
-        <v>176</v>
+        <v>0</v>
       </c>
       <c r="C84" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D84" t="s">
-        <v>5</v>
+        <v>171</v>
       </c>
       <c r="E84" t="s">
-        <v>38</v>
+        <v>172</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>175</v>
+        <v>33</v>
       </c>
       <c r="B85" t="s">
-        <v>178</v>
+        <v>0</v>
       </c>
       <c r="C85" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="D85" t="s">
-        <v>5</v>
+        <v>173</v>
       </c>
       <c r="E85" t="s">
-        <v>38</v>
+        <v>174</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>180</v>
+        <v>33</v>
       </c>
       <c r="B87" t="s">
-        <v>181</v>
+        <v>0</v>
       </c>
       <c r="C87" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D87" t="s">
-        <v>5</v>
+        <v>176</v>
       </c>
       <c r="E87" t="s">
-        <v>38</v>
+        <v>177</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>183</v>
+        <v>33</v>
       </c>
       <c r="B89" t="s">
-        <v>184</v>
+        <v>0</v>
       </c>
       <c r="C89" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D89" t="s">
-        <v>5</v>
+        <v>179</v>
       </c>
       <c r="E89" t="s">
-        <v>38</v>
+        <v>180</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>183</v>
+        <v>33</v>
       </c>
       <c r="B90" t="s">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="C90" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D90" t="s">
-        <v>5</v>
+        <v>181</v>
       </c>
       <c r="E90" t="s">
-        <v>38</v>
+        <v>182</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>188</v>
+        <v>33</v>
       </c>
       <c r="B92" t="s">
-        <v>189</v>
+        <v>0</v>
       </c>
       <c r="C92" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="D92" t="s">
-        <v>5</v>
+        <v>184</v>
       </c>
       <c r="E92" t="s">
-        <v>38</v>
+        <v>185</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>191</v>
+        <v>33</v>
       </c>
       <c r="B94" t="s">
-        <v>192</v>
+        <v>0</v>
       </c>
       <c r="C94" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="D94" t="s">
-        <v>5</v>
+        <v>187</v>
       </c>
       <c r="E94" t="s">
-        <v>38</v>
+        <v>188</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>191</v>
+        <v>33</v>
       </c>
       <c r="B95" t="s">
-        <v>194</v>
+        <v>0</v>
       </c>
       <c r="C95" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="D95" t="s">
-        <v>5</v>
+        <v>189</v>
       </c>
       <c r="E95" t="s">
-        <v>38</v>
+        <v>190</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>196</v>
+        <v>33</v>
       </c>
       <c r="B97" t="s">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="C97" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="D97" t="s">
-        <v>5</v>
+        <v>192</v>
       </c>
       <c r="E97" t="s">
-        <v>38</v>
+        <v>193</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>196</v>
+        <v>33</v>
       </c>
       <c r="B98" t="s">
-        <v>199</v>
+        <v>0</v>
       </c>
       <c r="C98" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D98" t="s">
-        <v>5</v>
+        <v>194</v>
       </c>
       <c r="E98" t="s">
-        <v>38</v>
+        <v>195</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>201</v>
+        <v>33</v>
       </c>
       <c r="B100" t="s">
-        <v>202</v>
+        <v>0</v>
       </c>
       <c r="C100" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="D100" t="s">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="E100" t="s">
-        <v>38</v>
+        <v>198</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>201</v>
+        <v>33</v>
       </c>
       <c r="B101" t="s">
-        <v>204</v>
+        <v>0</v>
       </c>
       <c r="C101" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="D101" t="s">
-        <v>5</v>
+        <v>199</v>
       </c>
       <c r="E101" t="s">
-        <v>38</v>
+        <v>200</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>206</v>
+        <v>33</v>
       </c>
       <c r="B103" t="s">
-        <v>207</v>
+        <v>0</v>
       </c>
       <c r="C103" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="D103" t="s">
-        <v>5</v>
+        <v>202</v>
       </c>
       <c r="E103" t="s">
-        <v>38</v>
+        <v>203</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>209</v>
+        <v>33</v>
       </c>
       <c r="B105" t="s">
-        <v>210</v>
+        <v>0</v>
       </c>
       <c r="C105" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="D105" t="s">
-        <v>5</v>
+        <v>205</v>
       </c>
       <c r="E105" t="s">
-        <v>38</v>
+        <v>206</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>209</v>
+        <v>33</v>
       </c>
       <c r="B106" t="s">
-        <v>212</v>
+        <v>0</v>
       </c>
       <c r="C106" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="D106" t="s">
-        <v>5</v>
+        <v>207</v>
       </c>
       <c r="E106" t="s">
-        <v>38</v>
+        <v>208</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>214</v>
+        <v>33</v>
       </c>
       <c r="B108" t="s">
-        <v>215</v>
+        <v>0</v>
       </c>
       <c r="C108" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D108" t="s">
-        <v>5</v>
+        <v>210</v>
       </c>
       <c r="E108" t="s">
-        <v>38</v>
+        <v>211</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>214</v>
+        <v>33</v>
       </c>
       <c r="B109" t="s">
-        <v>217</v>
+        <v>0</v>
       </c>
       <c r="C109" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D109" t="s">
-        <v>5</v>
+        <v>212</v>
       </c>
       <c r="E109" t="s">
-        <v>38</v>
+        <v>213</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>219</v>
+        <v>33</v>
       </c>
       <c r="B111" t="s">
-        <v>220</v>
+        <v>0</v>
       </c>
       <c r="C111" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D111" t="s">
-        <v>5</v>
+        <v>215</v>
       </c>
       <c r="E111" t="s">
-        <v>38</v>
+        <v>216</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>219</v>
+        <v>33</v>
       </c>
       <c r="B112" t="s">
-        <v>222</v>
+        <v>0</v>
       </c>
       <c r="C112" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D112" t="s">
-        <v>5</v>
+        <v>217</v>
       </c>
       <c r="E112" t="s">
-        <v>38</v>
+        <v>218</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>224</v>
+        <v>33</v>
       </c>
       <c r="B114" t="s">
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="C114" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="D114" t="s">
-        <v>5</v>
+        <v>220</v>
       </c>
       <c r="E114" t="s">
-        <v>38</v>
+        <v>221</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>224</v>
+        <v>33</v>
       </c>
       <c r="B115" t="s">
-        <v>227</v>
+        <v>0</v>
       </c>
       <c r="C115" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="D115" t="s">
-        <v>5</v>
+        <v>222</v>
       </c>
       <c r="E115" t="s">
-        <v>38</v>
+        <v>223</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>229</v>
+        <v>33</v>
       </c>
       <c r="B117" t="s">
-        <v>230</v>
+        <v>0</v>
       </c>
       <c r="C117" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="D117" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
       <c r="E117" t="s">
-        <v>38</v>
+        <v>226</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>229</v>
+        <v>33</v>
       </c>
       <c r="B118" t="s">
-        <v>232</v>
+        <v>0</v>
       </c>
       <c r="C118" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="D118" t="s">
-        <v>5</v>
+        <v>227</v>
       </c>
       <c r="E118" t="s">
-        <v>38</v>
+        <v>228</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>234</v>
+        <v>33</v>
       </c>
       <c r="B120" t="s">
-        <v>235</v>
+        <v>0</v>
       </c>
       <c r="C120" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="D120" t="s">
-        <v>5</v>
+        <v>230</v>
       </c>
       <c r="E120" t="s">
-        <v>38</v>
+        <v>231</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>234</v>
+        <v>33</v>
       </c>
       <c r="B121" t="s">
-        <v>237</v>
+        <v>0</v>
       </c>
       <c r="C121" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="D121" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E121" t="s">
-        <v>38</v>
+        <v>233</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>239</v>
+        <v>33</v>
       </c>
       <c r="B123" t="s">
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="C123" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="D123" t="s">
-        <v>5</v>
+        <v>235</v>
       </c>
       <c r="E123" t="s">
-        <v>38</v>
+        <v>236</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>242</v>
+        <v>33</v>
       </c>
       <c r="B125" t="s">
-        <v>243</v>
+        <v>0</v>
       </c>
       <c r="C125" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="D125" t="s">
-        <v>5</v>
+        <v>238</v>
       </c>
       <c r="E125" t="s">
-        <v>38</v>
+        <v>239</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>245</v>
+        <v>33</v>
       </c>
       <c r="B127" t="s">
-        <v>246</v>
+        <v>0</v>
       </c>
       <c r="C127" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="D127" t="s">
-        <v>5</v>
+        <v>241</v>
       </c>
       <c r="E127" t="s">
-        <v>38</v>
+        <v>242</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>245</v>
+        <v>33</v>
       </c>
       <c r="B128" t="s">
-        <v>248</v>
+        <v>0</v>
       </c>
       <c r="C128" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="D128" t="s">
-        <v>5</v>
+        <v>243</v>
       </c>
       <c r="E128" t="s">
-        <v>38</v>
+        <v>244</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>250</v>
+        <v>33</v>
       </c>
       <c r="B130" t="s">
-        <v>251</v>
+        <v>0</v>
       </c>
       <c r="C130" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="D130" t="s">
-        <v>5</v>
+        <v>246</v>
       </c>
       <c r="E130" t="s">
-        <v>38</v>
+        <v>247</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>253</v>
+        <v>33</v>
       </c>
       <c r="B132" t="s">
-        <v>254</v>
+        <v>0</v>
       </c>
       <c r="C132" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="D132" t="s">
-        <v>5</v>
+        <v>249</v>
       </c>
       <c r="E132" t="s">
-        <v>38</v>
+        <v>250</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>253</v>
+        <v>33</v>
       </c>
       <c r="B133" t="s">
-        <v>256</v>
+        <v>0</v>
       </c>
       <c r="C133" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="D133" t="s">
-        <v>5</v>
+        <v>251</v>
       </c>
       <c r="E133" t="s">
-        <v>38</v>
+        <v>252</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B134" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C134" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D134" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E134" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B135" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C135" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D135" t="s">
         <v>5</v>
@@ -2689,189 +2689,189 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
+        <v>1</v>
+      </c>
+      <c r="B136" t="s">
+        <v>0</v>
+      </c>
+      <c r="C136" t="s">
+        <v>2</v>
+      </c>
+      <c r="D136" t="s">
         <v>7</v>
       </c>
-      <c r="B136" t="s">
-        <v>12</v>
-      </c>
-      <c r="C136" t="s">
-        <v>13</v>
-      </c>
-      <c r="D136" t="s">
-        <v>5</v>
-      </c>
       <c r="E136" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B137" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C137" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D137" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E137" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B138" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C138" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D138" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E138" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B139" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C139" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D139" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E139" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B140" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C140" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D140" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E140" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B141" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="C141" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D141" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E141" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B142" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C142" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D142" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E142" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
+        <v>1</v>
+      </c>
+      <c r="B143" t="s">
+        <v>0</v>
+      </c>
+      <c r="C143" t="s">
+        <v>17</v>
+      </c>
+      <c r="D143" t="s">
         <v>22</v>
       </c>
-      <c r="B143" t="s">
-        <v>27</v>
-      </c>
-      <c r="C143" t="s">
-        <v>28</v>
-      </c>
-      <c r="D143" t="s">
-        <v>5</v>
-      </c>
       <c r="E143" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B144" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="C144" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D144" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="E144" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B145" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="C145" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D145" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="E145" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B146" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="C146" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D146" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="E146" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>